<commit_message>
fixed jours de ramasse, basic cli, refactoring
</commit_message>
<xml_diff>
--- a/data/points_de_ramasse.xlsx
+++ b/data/points_de_ramasse.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\ubuntu\home\pierre\routage-du-coeur\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A73C48-959E-4DA7-A307-4E5197D16720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Points de Ramasse"/>
+    <sheet name="Points de Ramasse" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Nom</t>
   </si>
@@ -28,9 +34,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Fréquence de Ramasse(/w)</t>
-  </si>
-  <si>
     <t>METRO</t>
   </si>
   <si>
@@ -71,13 +74,33 @@
   </si>
   <si>
     <t>1 Rue du Dr Charcot, 31830 Plaisance-du-Touch</t>
+  </si>
+  <si>
+    <t>Lundi, Mardi, Mercredi, Jeudi, Vendredi</t>
+  </si>
+  <si>
+    <t>Jours de Ramasse S1</t>
+  </si>
+  <si>
+    <t>Jours de Ramasse S2</t>
+  </si>
+  <si>
+    <t>Lundi, Mardi, Mercredi, Vendredi</t>
+  </si>
+  <si>
+    <t>Mercredi, Vendredi</t>
+  </si>
+  <si>
+    <t>Lundi, Jeudi, Vendredi</t>
+  </si>
+  <si>
+    <t>Mercredi, Mercredi(PL), Vendredi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,38 +158,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -177,10 +195,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -218,71 +236,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -310,7 +328,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -333,11 +351,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -346,13 +364,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -362,7 +380,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -371,7 +389,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -380,7 +398,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -388,10 +406,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -456,24 +474,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,127 +506,157 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3">
+        <v>43.643103500000002</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.4160820999999999</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4">
-        <v>43.6431035</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.4160821</v>
-      </c>
-      <c r="E2" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3">
+        <v>43.631926100000001</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.4843222</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
-        <v>43.6319261</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.4843222</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3">
+        <v>43.566146600000003</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.5171659</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
-        <v>43.5661466</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.5171659</v>
-      </c>
-      <c r="E4" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3">
+        <v>43.586419100000001</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.5776498000000001</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
-        <v>43.5864191</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.5776498</v>
-      </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3">
+        <v>43.644587999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.3726111000000001</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4">
-        <v>43.644588</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.3726111</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3">
+        <v>43.666604599999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.5141610000000001</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4">
-        <v>43.6666046</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.514161</v>
-      </c>
-      <c r="E7" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4">
-        <v>43.5913663</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="3">
+        <v>43.591366299999997</v>
+      </c>
+      <c r="D8" s="3">
         <v>1.2960563</v>
       </c>
-      <c r="E8" s="5">
-        <v>2</v>
-      </c>
+      <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Time windows, surgelés, data adjustments
</commit_message>
<xml_diff>
--- a/data/points_de_ramasse.xlsx
+++ b/data/points_de_ramasse.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Nom</t>
   </si>
@@ -28,10 +28,7 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Jours de Ramasse S1</t>
-  </si>
-  <si>
-    <t>Jours de Ramasse S2</t>
+    <t>Jours de Ramasse</t>
   </si>
   <si>
     <t>Poids par ramasse(kg)</t>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t>1 Rue du Dr Charcot, 31830 Plaisance-du-Touch</t>
-  </si>
-  <si>
-    <t>Mercredi, Mercredi(PL), Vendredi</t>
   </si>
 </sst>
 </file>
@@ -498,7 +492,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -509,8 +503,7 @@
     <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="10" width="42.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="42.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="18.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -529,19 +522,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="5">
         <v>43.6319261</v>
@@ -550,21 +540,18 @@
         <v>1.4843222</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="7">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7">
         <v>230</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>43.5661466</v>
@@ -573,21 +560,18 @@
         <v>1.5171659</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="7">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7">
         <v>250</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="5">
         <v>43.5864191</v>
@@ -596,21 +580,18 @@
         <v>1.5776498</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="7">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7">
         <v>210</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="5">
         <v>43.644588</v>
@@ -619,21 +600,18 @@
         <v>1.3726111</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="7">
+        <v>16</v>
+      </c>
+      <c r="F5" s="7">
         <v>230</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C6" s="5">
         <v>43.6666046</v>
@@ -642,21 +620,18 @@
         <v>1.514161</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="7">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7">
         <v>450</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C7" s="5">
         <v>43.5913663</v>
@@ -665,12 +640,9 @@
         <v>1.2960563</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="7">
+        <v>8</v>
+      </c>
+      <c r="F7" s="7">
         <v>800</v>
       </c>
     </row>

</xml_diff>

<commit_message>
major refactoring with new constraints
</commit_message>
<xml_diff>
--- a/data/points_de_ramasse.xlsx
+++ b/data/points_de_ramasse.xlsx
@@ -37,7 +37,7 @@
     <t>Type de produits</t>
   </si>
   <si>
-    <t>Auchan Gramont</t>
+    <t>AUCHAN GRAMONT</t>
   </si>
   <si>
     <t>Auchan Hypermarché Toulouse</t>
@@ -49,7 +49,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>Leclerc St Orens</t>
+    <t>LECLERC ST ORENS</t>
   </si>
   <si>
     <t>5 All. des Champs Pinsons, 31650 Saint-Orens-de-Gameville</t>
@@ -58,13 +58,13 @@
     <t>Lundi, Mardi, Mercredi, Jeudi, Vendredi</t>
   </si>
   <si>
-    <t>Super U Flourens</t>
+    <t>SUPER U FLOURENS</t>
   </si>
   <si>
     <t>Impasse du Moussard, 826 Rte de Castres D, 31130 Flourens</t>
   </si>
   <si>
-    <t>Leclerc Blagnac</t>
+    <t>LECLERC BLAGNAC</t>
   </si>
   <si>
     <t>2 All. Emile Zola, 31715 Blagnac</t>
@@ -73,22 +73,22 @@
     <t>Lundi, Jeudi, Vendredi</t>
   </si>
   <si>
-    <t>Leclerc Rouffiac</t>
-  </si>
-  <si>
-    <t>RD, 888 Rte d'Albi, 31180 Rouffiac-Tolosan</t>
+    <t>LECLERC ROUFFIAC</t>
+  </si>
+  <si>
+    <t>RD, 888 Rte d&amp;apos;Albi, 31180 Rouffiac-Tolosan</t>
   </si>
   <si>
     <t>Lundi, Mardi, Mercredi, Vendredi</t>
   </si>
   <si>
-    <t>Carrefour Supply Chain</t>
+    <t>CARREFOUR LA MENUDE</t>
   </si>
   <si>
     <t>1 Rue du Dr Charcot, 31830 Plaisance-du-Touch</t>
   </si>
   <si>
-    <t>Carrefour Supply Chain (A)</t>
+    <t>CARREFOUR EN JACCA</t>
   </si>
   <si>
     <t>Mercredi</t>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,24 +187,27 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -212,6 +215,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -236,31 +242,31 @@
         <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr lastClr="ffffff" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="1f497d"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="eeece1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -522,16 +528,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="27.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="42.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="27.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="42.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,168 +556,168 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>43.6319261</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>1.4843222</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <v>230</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>43.5661466</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>1.5171659</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="8">
         <v>250</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>43.5864191</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>1.5776498</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <v>210</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>43.644588</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>1.3726111</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="8">
         <v>230</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>43.6666046</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>1.514161</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="8">
         <v>450</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>43.5913663</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>1.2960563</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8">
         <v>800</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>43.5913663</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>1.2960563</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="8">
         <v>8000</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="9" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some more work on new data
</commit_message>
<xml_diff>
--- a/data/points_de_ramasse.xlsx
+++ b/data/points_de_ramasse.xlsx
@@ -79,7 +79,7 @@
     <t>RD, 888 Rte d&amp;apos;Albi, 31180 Rouffiac-Tolosan</t>
   </si>
   <si>
-    <t>Lundi, Mardi, Mercredi, Vendredi</t>
+    <t>Lundi, Mercredi, Vendredi</t>
   </si>
   <si>
     <t>CARREFOUR LA MENUDE</t>
@@ -102,7 +102,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,12 +113,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -176,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,15 +184,12 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -206,13 +197,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -528,16 +516,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="27.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="42.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="27.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="42.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="18.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,13 +561,13 @@
       <c r="D2" s="6">
         <v>1.4843222</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>230</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -596,13 +584,13 @@
       <c r="D3" s="6">
         <v>1.5171659</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>250</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -619,13 +607,13 @@
       <c r="D4" s="6">
         <v>1.5776498</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>210</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -642,13 +630,13 @@
       <c r="D5" s="6">
         <v>1.3726111</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>230</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -665,13 +653,13 @@
       <c r="D6" s="6">
         <v>1.514161</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>450</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -688,13 +676,13 @@
       <c r="D7" s="6">
         <v>1.2960563</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>800</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -711,13 +699,13 @@
       <c r="D8" s="6">
         <v>1.2960563</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>8000</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>